<commit_message>
files from multiple sessions are committed.
</commit_message>
<xml_diff>
--- a/class_related/061823-topic-on-python-classes/data/round_robin_matches_tabulation.xlsx
+++ b/class_related/061823-topic-on-python-classes/data/round_robin_matches_tabulation.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitrepos\becoming-cloud-engineer\class_related\061823-topic-on-python-classes\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCDFD32A-9817-44CE-9059-8DF78E6E11DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F05EBE5-77E5-4132-9970-D80651EA9D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A5975C6A-554B-48E0-87B4-80A7C5A3682B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="73">
   <si>
     <t>Team</t>
   </si>
@@ -60,13 +62,208 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>SG -Carlsen</t>
+  </si>
+  <si>
+    <t>GG - Anand</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>ssm1</t>
+  </si>
+  <si>
+    <t>ssm2</t>
+  </si>
+  <si>
+    <t>ssw1</t>
+  </si>
+  <si>
+    <t>ssw2</t>
+  </si>
+  <si>
+    <t>prodigy</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>SG - Won</t>
+  </si>
+  <si>
+    <t>Points - SG</t>
+  </si>
+  <si>
+    <t>Points - GG</t>
+  </si>
+  <si>
+    <t>Drawn</t>
+  </si>
+  <si>
+    <t>GG Won</t>
+  </si>
+  <si>
+    <t>Total Points</t>
+  </si>
+  <si>
+    <t>SG - Match Point</t>
+  </si>
+  <si>
+    <t>GG Match - Point</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>t2</t>
+  </si>
+  <si>
+    <t>t3</t>
+  </si>
+  <si>
+    <t>t4</t>
+  </si>
+  <si>
+    <t>t5</t>
+  </si>
+  <si>
+    <t>t6</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>p3</t>
+  </si>
+  <si>
+    <t>p4</t>
+  </si>
+  <si>
+    <t>p5</t>
+  </si>
+  <si>
+    <t>p6</t>
+  </si>
+  <si>
+    <t>p7</t>
+  </si>
+  <si>
+    <t>p8</t>
+  </si>
+  <si>
+    <t>p9</t>
+  </si>
+  <si>
+    <t>p10</t>
+  </si>
+  <si>
+    <t>p11</t>
+  </si>
+  <si>
+    <t>p12</t>
+  </si>
+  <si>
+    <t>p13</t>
+  </si>
+  <si>
+    <t>p14</t>
+  </si>
+  <si>
+    <t>p15</t>
+  </si>
+  <si>
+    <t>p16</t>
+  </si>
+  <si>
+    <t>p17</t>
+  </si>
+  <si>
+    <t>p18</t>
+  </si>
+  <si>
+    <t>p19</t>
+  </si>
+  <si>
+    <t>p20</t>
+  </si>
+  <si>
+    <t>p21</t>
+  </si>
+  <si>
+    <t>p22</t>
+  </si>
+  <si>
+    <t>p23</t>
+  </si>
+  <si>
+    <t>p24</t>
+  </si>
+  <si>
+    <t>p25</t>
+  </si>
+  <si>
+    <t>p26</t>
+  </si>
+  <si>
+    <t>p27</t>
+  </si>
+  <si>
+    <t>p28</t>
+  </si>
+  <si>
+    <t>p29</t>
+  </si>
+  <si>
+    <t>p30</t>
+  </si>
+  <si>
+    <t>p31</t>
+  </si>
+  <si>
+    <t>p32</t>
+  </si>
+  <si>
+    <t>p33</t>
+  </si>
+  <si>
+    <t>p34</t>
+  </si>
+  <si>
+    <t>p35</t>
+  </si>
+  <si>
+    <t>p36</t>
+  </si>
+  <si>
+    <t>TO1</t>
+  </si>
+  <si>
+    <t>TO2</t>
+  </si>
+  <si>
+    <t>TO3</t>
+  </si>
+  <si>
+    <t>TO4</t>
+  </si>
+  <si>
+    <t>TO5</t>
+  </si>
+  <si>
+    <t>TO6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,8 +279,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -93,6 +326,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -109,10 +354,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,7 +679,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,4 +842,575 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5251CE9B-B829-4CB6-8EF7-6AED7F543A4B}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="6">
+        <f>SUM(D2:D7)</f>
+        <v>6</v>
+      </c>
+      <c r="E8" s="6">
+        <f>SUM(E2:E7)</f>
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE16824B-1281-4401-B585-385820AE2A01}">
+  <dimension ref="A1:I66"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>69</v>
+      </c>
+      <c r="I15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" t="s">
+        <v>70</v>
+      </c>
+      <c r="I22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
+        <v>71</v>
+      </c>
+      <c r="I29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" t="s">
+        <v>72</v>
+      </c>
+      <c r="I36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>61</v>
+      </c>
+      <c r="I37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>62</v>
+      </c>
+      <c r="I38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>63</v>
+      </c>
+      <c r="I39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>64</v>
+      </c>
+      <c r="I40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>65</v>
+      </c>
+      <c r="I41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>66</v>
+      </c>
+      <c r="I42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I49" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I50" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I51" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I52" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I53" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I54" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I55" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I56" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I57" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I58" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I59" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I60" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I61" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I62" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I63" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I64" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I65" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I66" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>